<commit_message>
muchos cambios, informe8 ok
</commit_message>
<xml_diff>
--- a/informe.xlsx
+++ b/informe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\infDef_python\informes_defender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF56AA70-9AEE-445E-B06A-4C89B51472DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA05AD03-9DE0-4294-889D-D59D6245AB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13620" yWindow="-12690" windowWidth="13740" windowHeight="23790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MITIGACION" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="78">
   <si>
     <t>DeviceName</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>alejandro.cornejo</t>
+  </si>
+  <si>
+    <t>eduardo.XXXXXXXX</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1100,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A26" sqref="A26:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,7 +1917,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
         <v>54</v>
@@ -1946,7 +1949,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
         <v>55</v>
@@ -1978,7 +1981,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
@@ -2010,7 +2013,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
         <v>58</v>
@@ -2042,7 +2045,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
@@ -2074,7 +2077,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>

</xml_diff>